<commit_message>
Atualização de requisitos, atulização de Caso de Uso e adicioncando fluxo de caso de uso
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FATEC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A26FE0-E3E2-46A3-8A1E-FBBAE4DD4FBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Detalhado</t>
   </si>
@@ -103,12 +102,18 @@
   </si>
   <si>
     <t>RF6: O usuario poderá comparar a diferença de salarios, projetos aprovado e em trâmite(em andamento) dos politicos selecionados para comparação</t>
+  </si>
+  <si>
+    <t>RF9: Comparação de funcionários publicos</t>
+  </si>
+  <si>
+    <t>RF9: O usuario poderá comparar a diferença de salarios, dos funcionários selecionados para comparação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,11 +433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +530,12 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">

</xml_diff>

<commit_message>
Correção ortográfica de todos os documentos
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FATEC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FATEC\Desktop\Engenharia\pensabemapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,95 +29,102 @@
     <t>Detalhado</t>
   </si>
   <si>
-    <t xml:space="preserve">Surpeficiais </t>
-  </si>
-  <si>
-    <t>funcional</t>
-  </si>
-  <si>
-    <t>RF1 : Pesquisa com filtragem</t>
-  </si>
-  <si>
-    <t>RF2: Mostrar dados em forma de graficos</t>
-  </si>
-  <si>
-    <t>RF3: Histórico de politicos</t>
-  </si>
-  <si>
     <t>Não funcionais</t>
   </si>
   <si>
-    <t>RNF3:dados atualizados</t>
-  </si>
-  <si>
-    <t>RNF1:interface amigavel e simples</t>
-  </si>
-  <si>
-    <t>RNF2:aplicação rapida</t>
-  </si>
-  <si>
-    <t>RFN1: os usuarios são de todas as idades, portanto, quanto mais amigavel e simples, mais facil sera o uso do site.</t>
-  </si>
-  <si>
-    <t>RFN3: é de extrema importancia dados atualizados para manter o usuario bem informado</t>
-  </si>
-  <si>
-    <t>RFN2: para evitar estresse do usuario, a aplicação deve ser rapida</t>
-  </si>
-  <si>
-    <t>RF4: Mostrar dados em forma de tabela</t>
-  </si>
-  <si>
-    <t>RF4: Para pesquisa simples(como um salario de um servidor publico especifico), com o objetivo de facil entendimento, será demonstrado o resultado em forma de tabela</t>
-  </si>
-  <si>
-    <t>RF5: Busca de dados de servidores publicos</t>
-  </si>
-  <si>
-    <t>RF6: Comparação de politicos</t>
-  </si>
-  <si>
-    <t>RF1: O usuario pode realizar pesquisas especificas de acordo com os seguintes dados: salarios, cargos, nomes, projetos e tempo de serviço</t>
-  </si>
-  <si>
-    <t>RF3: O usuario poderá visualizar todos os dados dos politicos como projetos aprovados, salario,tempo de serviço, nome completo, idade e partido</t>
-  </si>
-  <si>
-    <t>RF7: Média e mediana de salários</t>
-  </si>
-  <si>
-    <t>RF5: Os dados devem ser buscados dos servidores publicos(Site da Prefeitura e da Câmara de Mogi das Cruzes), pois de acordo com a lei da transparecia, esses dados são oficiais e publicados pela propria prefeitura</t>
-  </si>
-  <si>
-    <t>RF2: O sistema mostra os dados em forma de gráfico para facil visualização e identificação da informação.Gráfico de barras para faixas salariais e gráfico de pizza para porcentagens.</t>
-  </si>
-  <si>
-    <t>RF8: Mostrar dados de funcionarios publicos</t>
-  </si>
-  <si>
-    <t>RF8: Será apresentado os seguintes dados dos funcionários publicos: Nome, cargo, remuneração, data da atualização do dado, regime, total bruto, total líquido e  total de desconto</t>
-  </si>
-  <si>
-    <t>RF7: Será apresentado a média e mediana de faixas salariais assim como apresentará o maior salario e o menor da faixa salarial de um cargo especifico</t>
-  </si>
-  <si>
-    <t>RF6: O usuario poderá comparar a diferença de salarios, projetos aprovado e em trâmite(em andamento) dos politicos selecionados para comparação</t>
-  </si>
-  <si>
-    <t>RF9: Comparação de funcionários publicos</t>
-  </si>
-  <si>
-    <t>RF9: O usuario poderá comparar a diferença de salarios, dos funcionários selecionados para comparação</t>
+    <t xml:space="preserve">Superficiais </t>
+  </si>
+  <si>
+    <t>Funcionais</t>
+  </si>
+  <si>
+    <t>RF1: Pesquisa com filtragem.</t>
+  </si>
+  <si>
+    <t>RF1: O usuário pode realizar pesquisas especificas de acordo com os seguintes dados: salários, cargos, nomes, projetos e tempo de serviço.</t>
+  </si>
+  <si>
+    <t>RF2: Mostrar dados em forma de gráficos.</t>
+  </si>
+  <si>
+    <t>RF2: O sistema mostra os dados em forma de gráfico para fácil visualização e identificação da informação. Gráfico de barras para faixas salariais e gráfico de pizza para porcentagens.</t>
+  </si>
+  <si>
+    <t>RF3: Histórico de políticos.</t>
+  </si>
+  <si>
+    <t>RF3: O usuário poderá visualizar todos os dados dos políticos como projetos aprovados, salario, tempo de serviço, nome completo, idade e partido.</t>
+  </si>
+  <si>
+    <t>RF4: Mostrar dados em forma de tabela.</t>
+  </si>
+  <si>
+    <t>RF4: Para pesquisa simples (como um salário de um servidor público especifico), com o objetivo de fácil entendimento, será demonstrado o resultado em forma de tabela.</t>
+  </si>
+  <si>
+    <t>RF5: Busca de dados de servidores públicos.</t>
+  </si>
+  <si>
+    <t>RF5: Os dados devem ser buscados dos servidores públicos (Site da Prefeitura e da Câmara de Mogi das Cruzes), pois de acordo com a lei da transparecia, esses dados são oficiais e publicados pela própria prefeitura.</t>
+  </si>
+  <si>
+    <t>RF6: Comparação de políticos.</t>
+  </si>
+  <si>
+    <t>RF6: O usuário poderá comparar a diferença de salários, projetos aprovado e em trâmite (em andamento) dos políticos selecionados para comparação.</t>
+  </si>
+  <si>
+    <t>RF7: Média e mediana de salários.</t>
+  </si>
+  <si>
+    <t>RF7: Será apresentado a média e mediana de faixas salariais assim como apresentará o maior salário e o menor da faixa salarial de um cargo especifico.</t>
+  </si>
+  <si>
+    <t>RF8: Mostrar dados de funcionários públicos.</t>
+  </si>
+  <si>
+    <t>RF8: Será apresentado os seguintes dados dos funcionários públicos: Nome, cargo, remuneração, data da atualização do dado, regime, total bruto, total líquido e total de desconto.</t>
+  </si>
+  <si>
+    <t>RF9: Comparação de funcionários públicos.</t>
+  </si>
+  <si>
+    <t>RF9: O usuário poderá comparar a diferença de salários, dos funcionários selecionados para comparação.</t>
+  </si>
+  <si>
+    <t>RNF1:interface amigável e simples.</t>
+  </si>
+  <si>
+    <t>RFN1: os usuários são de todas as idades, portanto, quanto mais amigável e simples, mais fácil será o uso do site.</t>
+  </si>
+  <si>
+    <t>RNF2:aplicação rápida.</t>
+  </si>
+  <si>
+    <t>RFN2: para evitar estresse do usuário, a aplicação deve ser rápida.</t>
+  </si>
+  <si>
+    <t>RNF3:dados atualizados.</t>
+  </si>
+  <si>
+    <t>RFN3: é de extrema importância dados atualizados para manter o usuário bem informado.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,15 +150,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -437,7 +447,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,140 +456,140 @@
     <col min="3" max="3" width="149.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" t="s">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>